<commit_message>
Gantt diagram frissitese (PHP --> NodeJS valtas)
</commit_message>
<xml_diff>
--- a/Gantt_diagram.xlsx
+++ b/Gantt_diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csiko\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1C1DEC-7FD3-4D35-AFE7-48BF3173CB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EC0CEF-863D-460C-A73A-A1FF77541EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1156,7 +1156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="208">
+  <cellXfs count="200">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1433,12 +1433,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="21" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1470,13 +1464,9 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="167" fontId="14" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1541,17 +1531,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1603,6 +1583,15 @@
     <xf numFmtId="0" fontId="18" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1616,15 +1605,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2132,11 +2112,11 @@
   </sheetPr>
   <dimension ref="A1:CL999"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="5" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="5" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomRight" activeCell="AK36" sqref="AK36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2145,7 +2125,7 @@
     <col min="2" max="2" width="58.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="2.7109375" customWidth="1"/>
     <col min="10" max="10" width="3.140625" customWidth="1"/>
     <col min="11" max="90" width="2.7109375" customWidth="1"/>
@@ -2160,85 +2140,85 @@
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
       <c r="H1" s="6"/>
-      <c r="I1" s="206" t="s">
+      <c r="I1" s="188" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="207"/>
-      <c r="K1" s="207"/>
-      <c r="L1" s="207"/>
-      <c r="M1" s="207"/>
-      <c r="N1" s="207"/>
-      <c r="O1" s="207"/>
-      <c r="P1" s="207"/>
+      <c r="J1" s="189"/>
+      <c r="K1" s="189"/>
+      <c r="L1" s="189"/>
+      <c r="M1" s="189"/>
+      <c r="N1" s="189"/>
+      <c r="O1" s="189"/>
+      <c r="P1" s="189"/>
       <c r="Q1" s="8"/>
-      <c r="R1" s="206" t="s">
+      <c r="R1" s="188" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="207"/>
-      <c r="T1" s="207"/>
-      <c r="U1" s="207"/>
-      <c r="V1" s="207"/>
+      <c r="S1" s="189"/>
+      <c r="T1" s="189"/>
+      <c r="U1" s="189"/>
+      <c r="V1" s="189"/>
       <c r="W1" s="9"/>
-      <c r="X1" s="206" t="s">
+      <c r="X1" s="188" t="s">
         <v>3</v>
       </c>
-      <c r="Y1" s="207"/>
-      <c r="Z1" s="207"/>
-      <c r="AA1" s="207"/>
-      <c r="AB1" s="207"/>
+      <c r="Y1" s="189"/>
+      <c r="Z1" s="189"/>
+      <c r="AA1" s="189"/>
+      <c r="AB1" s="189"/>
       <c r="AC1" s="10"/>
-      <c r="AD1" s="206" t="s">
+      <c r="AD1" s="188" t="s">
         <v>4</v>
       </c>
-      <c r="AE1" s="207"/>
-      <c r="AF1" s="207"/>
-      <c r="AG1" s="207"/>
-      <c r="AH1" s="207"/>
-      <c r="AI1" s="207"/>
-      <c r="AJ1" s="207"/>
-      <c r="AK1" s="207"/>
+      <c r="AE1" s="189"/>
+      <c r="AF1" s="189"/>
+      <c r="AG1" s="189"/>
+      <c r="AH1" s="189"/>
+      <c r="AI1" s="189"/>
+      <c r="AJ1" s="189"/>
+      <c r="AK1" s="189"/>
       <c r="AL1" s="11"/>
-      <c r="AM1" s="203" t="s">
+      <c r="AM1" s="190" t="s">
         <v>5</v>
       </c>
-      <c r="AN1" s="204"/>
-      <c r="AO1" s="204"/>
-      <c r="AP1" s="204"/>
-      <c r="AQ1" s="205"/>
+      <c r="AN1" s="191"/>
+      <c r="AO1" s="191"/>
+      <c r="AP1" s="191"/>
+      <c r="AQ1" s="192"/>
       <c r="AR1" s="12"/>
-      <c r="AS1" s="203" t="s">
+      <c r="AS1" s="190" t="s">
         <v>6</v>
       </c>
-      <c r="AT1" s="204"/>
-      <c r="AU1" s="204"/>
-      <c r="AV1" s="205"/>
+      <c r="AT1" s="191"/>
+      <c r="AU1" s="191"/>
+      <c r="AV1" s="192"/>
       <c r="AW1" s="13"/>
-      <c r="AX1" s="206" t="s">
+      <c r="AX1" s="188" t="s">
         <v>7</v>
       </c>
-      <c r="AY1" s="207"/>
-      <c r="AZ1" s="207"/>
-      <c r="BA1" s="207"/>
+      <c r="AY1" s="189"/>
+      <c r="AZ1" s="189"/>
+      <c r="BA1" s="189"/>
     </row>
     <row r="2" spans="1:90" ht="25.5" customHeight="1">
       <c r="A2" s="14"/>
       <c r="B2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="199" t="s">
+      <c r="D2" s="196" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="200"/>
+      <c r="E2" s="197"/>
       <c r="F2" s="5"/>
       <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:90" ht="25.5" customHeight="1">
       <c r="A3" s="14"/>
       <c r="B3" s="17"/>
-      <c r="D3" s="199">
+      <c r="D3" s="196">
         <v>45189</v>
       </c>
-      <c r="E3" s="200"/>
+      <c r="E3" s="197"/>
       <c r="F3" s="5"/>
       <c r="AC3" s="18" t="s">
         <v>10</v>
@@ -2255,127 +2235,127 @@
     </row>
     <row r="4" spans="1:90" ht="25.5" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="F4" s="201"/>
-      <c r="G4" s="196">
+      <c r="F4" s="198"/>
+      <c r="G4" s="193">
         <f>G5</f>
         <v>45187</v>
       </c>
-      <c r="H4" s="197"/>
-      <c r="I4" s="197"/>
-      <c r="J4" s="197"/>
-      <c r="K4" s="197"/>
-      <c r="L4" s="197"/>
-      <c r="M4" s="198"/>
-      <c r="N4" s="196">
+      <c r="H4" s="194"/>
+      <c r="I4" s="194"/>
+      <c r="J4" s="194"/>
+      <c r="K4" s="194"/>
+      <c r="L4" s="194"/>
+      <c r="M4" s="195"/>
+      <c r="N4" s="193">
         <f>N5</f>
         <v>45194</v>
       </c>
-      <c r="O4" s="197"/>
-      <c r="P4" s="197"/>
-      <c r="Q4" s="197"/>
-      <c r="R4" s="197"/>
-      <c r="S4" s="197"/>
-      <c r="T4" s="198"/>
-      <c r="U4" s="196">
+      <c r="O4" s="194"/>
+      <c r="P4" s="194"/>
+      <c r="Q4" s="194"/>
+      <c r="R4" s="194"/>
+      <c r="S4" s="194"/>
+      <c r="T4" s="195"/>
+      <c r="U4" s="193">
         <f>U5</f>
         <v>45201</v>
       </c>
-      <c r="V4" s="197"/>
-      <c r="W4" s="197"/>
-      <c r="X4" s="197"/>
-      <c r="Y4" s="197"/>
-      <c r="Z4" s="197"/>
-      <c r="AA4" s="198"/>
-      <c r="AB4" s="196">
+      <c r="V4" s="194"/>
+      <c r="W4" s="194"/>
+      <c r="X4" s="194"/>
+      <c r="Y4" s="194"/>
+      <c r="Z4" s="194"/>
+      <c r="AA4" s="195"/>
+      <c r="AB4" s="193">
         <f>AB5</f>
         <v>45208</v>
       </c>
-      <c r="AC4" s="197"/>
-      <c r="AD4" s="197"/>
-      <c r="AE4" s="197"/>
-      <c r="AF4" s="197"/>
-      <c r="AG4" s="197"/>
-      <c r="AH4" s="198"/>
-      <c r="AI4" s="196">
+      <c r="AC4" s="194"/>
+      <c r="AD4" s="194"/>
+      <c r="AE4" s="194"/>
+      <c r="AF4" s="194"/>
+      <c r="AG4" s="194"/>
+      <c r="AH4" s="195"/>
+      <c r="AI4" s="193">
         <f>AI5</f>
         <v>45215</v>
       </c>
-      <c r="AJ4" s="197"/>
-      <c r="AK4" s="197"/>
-      <c r="AL4" s="197"/>
-      <c r="AM4" s="197"/>
-      <c r="AN4" s="197"/>
-      <c r="AO4" s="198"/>
-      <c r="AP4" s="196">
+      <c r="AJ4" s="194"/>
+      <c r="AK4" s="194"/>
+      <c r="AL4" s="194"/>
+      <c r="AM4" s="194"/>
+      <c r="AN4" s="194"/>
+      <c r="AO4" s="195"/>
+      <c r="AP4" s="193">
         <f>AP5</f>
         <v>45222</v>
       </c>
-      <c r="AQ4" s="197"/>
-      <c r="AR4" s="197"/>
-      <c r="AS4" s="197"/>
-      <c r="AT4" s="197"/>
-      <c r="AU4" s="197"/>
-      <c r="AV4" s="198"/>
-      <c r="AW4" s="196">
+      <c r="AQ4" s="194"/>
+      <c r="AR4" s="194"/>
+      <c r="AS4" s="194"/>
+      <c r="AT4" s="194"/>
+      <c r="AU4" s="194"/>
+      <c r="AV4" s="195"/>
+      <c r="AW4" s="193">
         <f>AW5</f>
         <v>45229</v>
       </c>
-      <c r="AX4" s="197"/>
-      <c r="AY4" s="197"/>
-      <c r="AZ4" s="197"/>
-      <c r="BA4" s="197"/>
-      <c r="BB4" s="197"/>
-      <c r="BC4" s="198"/>
-      <c r="BD4" s="196">
+      <c r="AX4" s="194"/>
+      <c r="AY4" s="194"/>
+      <c r="AZ4" s="194"/>
+      <c r="BA4" s="194"/>
+      <c r="BB4" s="194"/>
+      <c r="BC4" s="195"/>
+      <c r="BD4" s="193">
         <f>BD5</f>
         <v>45236</v>
       </c>
-      <c r="BE4" s="197"/>
-      <c r="BF4" s="197"/>
-      <c r="BG4" s="197"/>
-      <c r="BH4" s="197"/>
-      <c r="BI4" s="197"/>
-      <c r="BJ4" s="198"/>
-      <c r="BK4" s="196">
+      <c r="BE4" s="194"/>
+      <c r="BF4" s="194"/>
+      <c r="BG4" s="194"/>
+      <c r="BH4" s="194"/>
+      <c r="BI4" s="194"/>
+      <c r="BJ4" s="195"/>
+      <c r="BK4" s="193">
         <f>BK5</f>
         <v>45243</v>
       </c>
-      <c r="BL4" s="197"/>
-      <c r="BM4" s="197"/>
-      <c r="BN4" s="197"/>
-      <c r="BO4" s="197"/>
-      <c r="BP4" s="197"/>
-      <c r="BQ4" s="198"/>
-      <c r="BR4" s="196">
+      <c r="BL4" s="194"/>
+      <c r="BM4" s="194"/>
+      <c r="BN4" s="194"/>
+      <c r="BO4" s="194"/>
+      <c r="BP4" s="194"/>
+      <c r="BQ4" s="195"/>
+      <c r="BR4" s="193">
         <f>BR5</f>
         <v>45250</v>
       </c>
-      <c r="BS4" s="197"/>
-      <c r="BT4" s="197"/>
-      <c r="BU4" s="197"/>
-      <c r="BV4" s="197"/>
-      <c r="BW4" s="197"/>
-      <c r="BX4" s="198"/>
-      <c r="BY4" s="196">
+      <c r="BS4" s="194"/>
+      <c r="BT4" s="194"/>
+      <c r="BU4" s="194"/>
+      <c r="BV4" s="194"/>
+      <c r="BW4" s="194"/>
+      <c r="BX4" s="195"/>
+      <c r="BY4" s="193">
         <f>BY5</f>
         <v>45257</v>
       </c>
-      <c r="BZ4" s="197"/>
-      <c r="CA4" s="197"/>
-      <c r="CB4" s="197"/>
-      <c r="CC4" s="197"/>
-      <c r="CD4" s="197"/>
-      <c r="CE4" s="198"/>
-      <c r="CF4" s="196">
+      <c r="BZ4" s="194"/>
+      <c r="CA4" s="194"/>
+      <c r="CB4" s="194"/>
+      <c r="CC4" s="194"/>
+      <c r="CD4" s="194"/>
+      <c r="CE4" s="195"/>
+      <c r="CF4" s="193">
         <f>CF5</f>
         <v>45264</v>
       </c>
-      <c r="CG4" s="197"/>
-      <c r="CH4" s="197"/>
-      <c r="CI4" s="197"/>
-      <c r="CJ4" s="197"/>
-      <c r="CK4" s="197"/>
-      <c r="CL4" s="198"/>
+      <c r="CG4" s="194"/>
+      <c r="CH4" s="194"/>
+      <c r="CI4" s="194"/>
+      <c r="CJ4" s="194"/>
+      <c r="CK4" s="194"/>
+      <c r="CL4" s="195"/>
     </row>
     <row r="5" spans="1:90" ht="25.5" customHeight="1" thickBot="1">
       <c r="A5" s="1"/>
@@ -2391,7 +2371,7 @@
       <c r="E5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="202"/>
+      <c r="F5" s="199"/>
       <c r="G5" s="21">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2</f>
         <v>45187</v>
@@ -2476,7 +2456,7 @@
         <f t="shared" si="0"/>
         <v>45207</v>
       </c>
-      <c r="AB5" s="181">
+      <c r="AB5" s="173">
         <f t="shared" si="0"/>
         <v>45208</v>
       </c>
@@ -2536,7 +2516,7 @@
         <f t="shared" si="0"/>
         <v>45222</v>
       </c>
-      <c r="AQ5" s="192">
+      <c r="AQ5" s="184">
         <f t="shared" si="0"/>
         <v>45223</v>
       </c>
@@ -2620,7 +2600,7 @@
         <f t="shared" si="0"/>
         <v>45243</v>
       </c>
-      <c r="BL5" s="192">
+      <c r="BL5" s="184">
         <f t="shared" si="0"/>
         <v>45244</v>
       </c>
@@ -2704,7 +2684,7 @@
         <f t="shared" si="0"/>
         <v>45264</v>
       </c>
-      <c r="CG5" s="192">
+      <c r="CG5" s="184">
         <f t="shared" si="0"/>
         <v>45265</v>
       </c>
@@ -2755,7 +2735,7 @@
       <c r="Z6" s="30"/>
       <c r="AA6" s="30"/>
       <c r="AB6" s="31"/>
-      <c r="AC6" s="191"/>
+      <c r="AC6" s="183"/>
       <c r="AD6" s="33"/>
       <c r="AE6" s="29"/>
       <c r="AF6" s="29"/>
@@ -2849,7 +2829,7 @@
       <c r="Z7" s="39"/>
       <c r="AA7" s="39"/>
       <c r="AB7" s="40"/>
-      <c r="AC7" s="184"/>
+      <c r="AC7" s="176"/>
       <c r="AD7" s="42"/>
       <c r="AE7" s="38"/>
       <c r="AF7" s="38"/>
@@ -2949,8 +2929,8 @@
       <c r="Y8" s="48"/>
       <c r="Z8" s="48"/>
       <c r="AA8" s="48"/>
-      <c r="AB8" s="182"/>
-      <c r="AC8" s="185"/>
+      <c r="AB8" s="174"/>
+      <c r="AC8" s="177"/>
       <c r="AD8" s="42"/>
       <c r="AE8" s="38"/>
       <c r="AF8" s="38"/>
@@ -3050,8 +3030,8 @@
       <c r="Y9" s="49"/>
       <c r="Z9" s="49"/>
       <c r="AA9" s="54"/>
-      <c r="AB9" s="183"/>
-      <c r="AC9" s="186"/>
+      <c r="AB9" s="175"/>
+      <c r="AC9" s="178"/>
       <c r="AD9" s="49"/>
       <c r="AE9" s="49"/>
       <c r="AF9" s="49"/>
@@ -3144,7 +3124,7 @@
       <c r="Y10" s="63"/>
       <c r="Z10" s="63"/>
       <c r="AA10" s="63"/>
-      <c r="AB10" s="152"/>
+      <c r="AB10" s="148"/>
       <c r="AC10" s="63"/>
       <c r="AD10" s="63"/>
       <c r="AE10" s="63"/>
@@ -3210,7 +3190,7 @@
     </row>
     <row r="11" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="193" t="s">
+      <c r="B11" s="185" t="s">
         <v>55</v>
       </c>
       <c r="C11" s="66" t="s">
@@ -3246,7 +3226,7 @@
       <c r="Z11" s="39"/>
       <c r="AA11" s="39"/>
       <c r="AB11" s="40"/>
-      <c r="AC11" s="187"/>
+      <c r="AC11" s="179"/>
       <c r="AD11" s="75"/>
       <c r="AE11" s="75"/>
       <c r="AF11" s="75"/>
@@ -3311,7 +3291,7 @@
     </row>
     <row r="12" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="193" t="s">
+      <c r="B12" s="185" t="s">
         <v>56</v>
       </c>
       <c r="C12" s="66" t="s">
@@ -3346,7 +3326,7 @@
       <c r="Z12" s="39"/>
       <c r="AA12" s="39"/>
       <c r="AB12" s="76"/>
-      <c r="AC12" s="188"/>
+      <c r="AC12" s="180"/>
       <c r="AD12" s="78"/>
       <c r="AE12" s="47"/>
       <c r="AF12" s="82"/>
@@ -3411,7 +3391,7 @@
     </row>
     <row r="13" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="193" t="s">
+      <c r="B13" s="185" t="s">
         <v>57</v>
       </c>
       <c r="C13" s="66" t="s">
@@ -3447,7 +3427,7 @@
       <c r="Z13" s="39"/>
       <c r="AA13" s="39"/>
       <c r="AB13" s="83"/>
-      <c r="AC13" s="184"/>
+      <c r="AC13" s="176"/>
       <c r="AD13" s="42"/>
       <c r="AE13" s="38"/>
       <c r="AF13" s="12"/>
@@ -3512,7 +3492,7 @@
     </row>
     <row r="14" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="193" t="s">
+      <c r="B14" s="185" t="s">
         <v>58</v>
       </c>
       <c r="C14" s="66" t="s">
@@ -3548,7 +3528,7 @@
       <c r="Z14" s="39"/>
       <c r="AA14" s="39"/>
       <c r="AB14" s="76"/>
-      <c r="AC14" s="188"/>
+      <c r="AC14" s="180"/>
       <c r="AD14" s="78"/>
       <c r="AE14" s="79"/>
       <c r="AF14" s="38"/>
@@ -3613,7 +3593,7 @@
     </row>
     <row r="15" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="193" t="s">
+      <c r="B15" s="185" t="s">
         <v>59</v>
       </c>
       <c r="C15" s="66" t="s">
@@ -3649,7 +3629,7 @@
       <c r="Z15" s="46"/>
       <c r="AA15" s="46"/>
       <c r="AB15" s="76"/>
-      <c r="AC15" s="184"/>
+      <c r="AC15" s="176"/>
       <c r="AD15" s="42"/>
       <c r="AE15" s="38"/>
       <c r="AF15" s="38"/>
@@ -3714,7 +3694,7 @@
     </row>
     <row r="16" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="193" t="s">
+      <c r="B16" s="185" t="s">
         <v>60</v>
       </c>
       <c r="C16" s="66" t="s">
@@ -3749,8 +3729,8 @@
       <c r="Y16" s="68"/>
       <c r="Z16" s="70"/>
       <c r="AA16" s="70"/>
-      <c r="AB16" s="155"/>
-      <c r="AC16" s="189"/>
+      <c r="AB16" s="151"/>
+      <c r="AC16" s="181"/>
       <c r="AD16" s="74"/>
       <c r="AE16" s="68"/>
       <c r="AF16" s="68"/>
@@ -3815,7 +3795,7 @@
     </row>
     <row r="17" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="193" t="s">
+      <c r="B17" s="185" t="s">
         <v>61</v>
       </c>
       <c r="C17" s="66" t="s">
@@ -3850,7 +3830,7 @@
       <c r="Z17" s="50"/>
       <c r="AA17" s="50"/>
       <c r="AB17" s="55"/>
-      <c r="AC17" s="190"/>
+      <c r="AC17" s="182"/>
       <c r="AD17" s="57"/>
       <c r="AE17" s="49"/>
       <c r="AF17" s="52"/>
@@ -4009,7 +3989,7 @@
     </row>
     <row r="19" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="194" t="s">
+      <c r="B19" s="186" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="95" t="s">
@@ -4045,7 +4025,7 @@
       <c r="Z19" s="39"/>
       <c r="AA19" s="39"/>
       <c r="AB19" s="40"/>
-      <c r="AC19" s="184"/>
+      <c r="AC19" s="176"/>
       <c r="AD19" s="42"/>
       <c r="AE19" s="38"/>
       <c r="AF19" s="38"/>
@@ -4110,7 +4090,7 @@
     </row>
     <row r="20" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="194" t="s">
+      <c r="B20" s="186" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="95" t="s">
@@ -4146,7 +4126,7 @@
       <c r="Z20" s="39"/>
       <c r="AA20" s="39"/>
       <c r="AB20" s="40"/>
-      <c r="AC20" s="184"/>
+      <c r="AC20" s="176"/>
       <c r="AD20" s="42"/>
       <c r="AE20" s="38"/>
       <c r="AF20" s="38"/>
@@ -4163,8 +4143,8 @@
       <c r="AQ20" s="41"/>
       <c r="AR20" s="42"/>
       <c r="AS20" s="9"/>
-      <c r="AT20" s="158"/>
-      <c r="AU20" s="158"/>
+      <c r="AT20" s="154"/>
+      <c r="AU20" s="154"/>
       <c r="AV20" s="9"/>
       <c r="AW20" s="47"/>
       <c r="AX20" s="47"/>
@@ -4211,7 +4191,7 @@
     </row>
     <row r="21" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="194" t="s">
+      <c r="B21" s="186" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="95" t="s">
@@ -4246,7 +4226,7 @@
       <c r="Z21" s="39"/>
       <c r="AA21" s="39"/>
       <c r="AB21" s="40"/>
-      <c r="AC21" s="184"/>
+      <c r="AC21" s="176"/>
       <c r="AD21" s="42"/>
       <c r="AE21" s="38"/>
       <c r="AF21" s="38"/>
@@ -4270,9 +4250,9 @@
       <c r="AX21" s="82"/>
       <c r="AY21" s="38"/>
       <c r="AZ21" s="40"/>
-      <c r="BA21" s="160"/>
-      <c r="BB21" s="160"/>
-      <c r="BC21" s="160"/>
+      <c r="BA21" s="156"/>
+      <c r="BB21" s="156"/>
+      <c r="BC21" s="156"/>
       <c r="BD21" s="42"/>
       <c r="BE21" s="38"/>
       <c r="BF21" s="38"/>
@@ -4311,7 +4291,7 @@
     </row>
     <row r="22" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="194" t="s">
+      <c r="B22" s="186" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="95" t="s">
@@ -4347,7 +4327,7 @@
       <c r="Z22" s="39"/>
       <c r="AA22" s="39"/>
       <c r="AB22" s="40"/>
-      <c r="AC22" s="184"/>
+      <c r="AC22" s="176"/>
       <c r="AD22" s="42"/>
       <c r="AE22" s="38"/>
       <c r="AF22" s="38"/>
@@ -4364,11 +4344,11 @@
       <c r="AQ22" s="41"/>
       <c r="AR22" s="42"/>
       <c r="AS22" s="76"/>
-      <c r="AT22" s="160"/>
-      <c r="AU22" s="160"/>
-      <c r="AV22" s="164"/>
-      <c r="AW22" s="158"/>
-      <c r="AX22" s="158"/>
+      <c r="AT22" s="156"/>
+      <c r="AU22" s="156"/>
+      <c r="AV22" s="160"/>
+      <c r="AW22" s="154"/>
+      <c r="AX22" s="154"/>
       <c r="AY22" s="47"/>
       <c r="AZ22" s="47"/>
       <c r="BA22" s="47"/>
@@ -4412,7 +4392,7 @@
     </row>
     <row r="23" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="194" t="s">
+      <c r="B23" s="186" t="s">
         <v>31</v>
       </c>
       <c r="C23" s="95" t="s">
@@ -4448,7 +4428,7 @@
       <c r="Z23" s="39"/>
       <c r="AA23" s="39"/>
       <c r="AB23" s="40"/>
-      <c r="AC23" s="184"/>
+      <c r="AC23" s="176"/>
       <c r="AD23" s="42"/>
       <c r="AE23" s="38"/>
       <c r="AF23" s="38"/>
@@ -4513,11 +4493,11 @@
     </row>
     <row r="24" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="194" t="s">
+      <c r="B24" s="186" t="s">
         <v>32</v>
       </c>
       <c r="C24" s="95" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D24" s="96">
         <v>45231</v>
@@ -4549,7 +4529,7 @@
       <c r="Z24" s="39"/>
       <c r="AA24" s="39"/>
       <c r="AB24" s="40"/>
-      <c r="AC24" s="184"/>
+      <c r="AC24" s="176"/>
       <c r="AD24" s="42"/>
       <c r="AE24" s="38"/>
       <c r="AF24" s="38"/>
@@ -4568,15 +4548,15 @@
       <c r="AS24" s="79"/>
       <c r="AT24" s="79"/>
       <c r="AU24" s="39"/>
-      <c r="AV24" s="169"/>
-      <c r="AW24" s="160"/>
-      <c r="AX24" s="160"/>
-      <c r="AY24" s="170"/>
-      <c r="AZ24" s="168"/>
-      <c r="BA24" s="81"/>
-      <c r="BB24" s="117"/>
-      <c r="BC24" s="117"/>
-      <c r="BD24" s="157"/>
+      <c r="AV24" s="164"/>
+      <c r="AW24" s="156"/>
+      <c r="AX24" s="156"/>
+      <c r="AY24" s="6"/>
+      <c r="AZ24" s="6"/>
+      <c r="BA24" s="6"/>
+      <c r="BB24" s="6"/>
+      <c r="BC24" s="6"/>
+      <c r="BD24" s="153"/>
       <c r="BE24" s="38"/>
       <c r="BF24" s="38"/>
       <c r="BG24" s="38"/>
@@ -4614,11 +4594,11 @@
     </row>
     <row r="25" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="194" t="s">
+      <c r="B25" s="186" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="95" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D25" s="96">
         <v>45231</v>
@@ -4650,7 +4630,7 @@
       <c r="Z25" s="39"/>
       <c r="AA25" s="39"/>
       <c r="AB25" s="40"/>
-      <c r="AC25" s="184"/>
+      <c r="AC25" s="176"/>
       <c r="AD25" s="42"/>
       <c r="AE25" s="38"/>
       <c r="AF25" s="38"/>
@@ -4667,19 +4647,19 @@
       <c r="AQ25" s="41"/>
       <c r="AR25" s="102"/>
       <c r="AS25" s="101"/>
-      <c r="AT25" s="165"/>
-      <c r="AU25" s="166"/>
-      <c r="AV25" s="160"/>
-      <c r="AW25" s="160"/>
-      <c r="AX25" s="160"/>
-      <c r="AY25" s="100"/>
-      <c r="AZ25" s="100"/>
-      <c r="BA25" s="100"/>
-      <c r="BB25" s="100"/>
-      <c r="BC25" s="100"/>
-      <c r="BD25" s="100"/>
-      <c r="BE25" s="100"/>
-      <c r="BF25" s="100"/>
+      <c r="AT25" s="161"/>
+      <c r="AU25" s="162"/>
+      <c r="AV25" s="156"/>
+      <c r="AW25" s="156"/>
+      <c r="AX25" s="156"/>
+      <c r="AY25" s="10"/>
+      <c r="AZ25" s="10"/>
+      <c r="BA25" s="10"/>
+      <c r="BB25" s="10"/>
+      <c r="BC25" s="10"/>
+      <c r="BD25" s="10"/>
+      <c r="BE25" s="10"/>
+      <c r="BF25" s="10"/>
       <c r="BG25" s="101"/>
       <c r="BH25" s="101"/>
       <c r="BI25" s="39"/>
@@ -4715,7 +4695,7 @@
     </row>
     <row r="26" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="194" t="s">
+      <c r="B26" s="186" t="s">
         <v>34</v>
       </c>
       <c r="C26" s="95" t="s">
@@ -4751,7 +4731,7 @@
       <c r="Z26" s="39"/>
       <c r="AA26" s="39"/>
       <c r="AB26" s="40"/>
-      <c r="AC26" s="184"/>
+      <c r="AC26" s="176"/>
       <c r="AD26" s="42"/>
       <c r="AE26" s="38"/>
       <c r="AF26" s="38"/>
@@ -4770,10 +4750,10 @@
       <c r="AS26" s="102"/>
       <c r="AT26" s="102"/>
       <c r="AU26" s="102"/>
-      <c r="AV26" s="167"/>
-      <c r="AW26" s="160"/>
-      <c r="AX26" s="160"/>
-      <c r="AY26" s="163"/>
+      <c r="AV26" s="163"/>
+      <c r="AW26" s="156"/>
+      <c r="AX26" s="156"/>
+      <c r="AY26" s="159"/>
       <c r="AZ26" s="75"/>
       <c r="BA26" s="75"/>
       <c r="BB26" s="75"/>
@@ -4816,7 +4796,7 @@
     </row>
     <row r="27" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="194" t="s">
+      <c r="B27" s="186" t="s">
         <v>35</v>
       </c>
       <c r="C27" s="95" t="s">
@@ -4852,7 +4832,7 @@
       <c r="Z27" s="39"/>
       <c r="AA27" s="39"/>
       <c r="AB27" s="40"/>
-      <c r="AC27" s="184"/>
+      <c r="AC27" s="176"/>
       <c r="AD27" s="42"/>
       <c r="AE27" s="38"/>
       <c r="AF27" s="38"/>
@@ -4873,7 +4853,7 @@
       <c r="AU27" s="39"/>
       <c r="AV27" s="39"/>
       <c r="AW27" s="51"/>
-      <c r="AX27" s="157"/>
+      <c r="AX27" s="153"/>
       <c r="AY27" s="38"/>
       <c r="AZ27" s="103"/>
       <c r="BA27" s="103"/>
@@ -4917,7 +4897,7 @@
     </row>
     <row r="28" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="194" t="s">
+      <c r="B28" s="186" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="95" t="s">
@@ -4953,7 +4933,7 @@
       <c r="Z28" s="39"/>
       <c r="AA28" s="39"/>
       <c r="AB28" s="40"/>
-      <c r="AC28" s="184"/>
+      <c r="AC28" s="176"/>
       <c r="AD28" s="42"/>
       <c r="AE28" s="38"/>
       <c r="AF28" s="38"/>
@@ -4972,12 +4952,12 @@
       <c r="AS28" s="47"/>
       <c r="AT28" s="79"/>
       <c r="AU28" s="39"/>
-      <c r="AV28" s="169"/>
-      <c r="AW28" s="174"/>
-      <c r="AX28" s="173"/>
+      <c r="AV28" s="164"/>
+      <c r="AW28" s="166"/>
+      <c r="AX28" s="165"/>
       <c r="AY28" s="42"/>
       <c r="AZ28" s="38"/>
-      <c r="BA28" s="153"/>
+      <c r="BA28" s="149"/>
       <c r="BB28" s="103"/>
       <c r="BC28" s="103"/>
       <c r="BD28" s="12"/>
@@ -5018,11 +4998,11 @@
     </row>
     <row r="29" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="194" t="s">
+      <c r="B29" s="186" t="s">
         <v>37</v>
       </c>
       <c r="C29" s="95" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D29" s="96">
         <v>45236</v>
@@ -5054,7 +5034,7 @@
       <c r="Z29" s="39"/>
       <c r="AA29" s="39"/>
       <c r="AB29" s="40"/>
-      <c r="AC29" s="184"/>
+      <c r="AC29" s="176"/>
       <c r="AD29" s="42"/>
       <c r="AE29" s="38"/>
       <c r="AF29" s="38"/>
@@ -5074,20 +5054,20 @@
       <c r="AT29" s="47"/>
       <c r="AU29" s="46"/>
       <c r="AV29" s="46"/>
-      <c r="AW29" s="154"/>
-      <c r="AX29" s="153"/>
+      <c r="AW29" s="150"/>
+      <c r="AX29" s="149"/>
       <c r="AY29" s="38"/>
       <c r="AZ29" s="38"/>
       <c r="BA29" s="38"/>
       <c r="BB29" s="69"/>
       <c r="BC29" s="69"/>
-      <c r="BD29" s="171"/>
-      <c r="BE29" s="100"/>
-      <c r="BF29" s="100"/>
-      <c r="BG29" s="100"/>
-      <c r="BH29" s="100"/>
-      <c r="BI29" s="100"/>
-      <c r="BJ29" s="100"/>
+      <c r="BD29" s="10"/>
+      <c r="BE29" s="10"/>
+      <c r="BF29" s="10"/>
+      <c r="BG29" s="10"/>
+      <c r="BH29" s="10"/>
+      <c r="BI29" s="10"/>
+      <c r="BJ29" s="10"/>
       <c r="BK29" s="101"/>
       <c r="BL29" s="41"/>
       <c r="BM29" s="42"/>
@@ -5119,7 +5099,7 @@
     </row>
     <row r="30" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="194" t="s">
+      <c r="B30" s="186" t="s">
         <v>38</v>
       </c>
       <c r="C30" s="95" t="s">
@@ -5155,7 +5135,7 @@
       <c r="Z30" s="39"/>
       <c r="AA30" s="39"/>
       <c r="AB30" s="40"/>
-      <c r="AC30" s="184"/>
+      <c r="AC30" s="176"/>
       <c r="AD30" s="42"/>
       <c r="AE30" s="38"/>
       <c r="AF30" s="38"/>
@@ -5220,11 +5200,11 @@
     </row>
     <row r="31" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A31" s="1"/>
-      <c r="B31" s="194" t="s">
+      <c r="B31" s="186" t="s">
         <v>39</v>
       </c>
       <c r="C31" s="95" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D31" s="96">
         <v>45237</v>
@@ -5256,7 +5236,7 @@
       <c r="Z31" s="39"/>
       <c r="AA31" s="39"/>
       <c r="AB31" s="40"/>
-      <c r="AC31" s="184"/>
+      <c r="AC31" s="176"/>
       <c r="AD31" s="42"/>
       <c r="AE31" s="38"/>
       <c r="AF31" s="38"/>
@@ -5275,20 +5255,20 @@
       <c r="AS31" s="47"/>
       <c r="AT31" s="47"/>
       <c r="AU31" s="46"/>
-      <c r="AV31" s="162"/>
-      <c r="AW31" s="175"/>
-      <c r="AX31" s="173"/>
+      <c r="AV31" s="158"/>
+      <c r="AW31" s="167"/>
+      <c r="AX31" s="165"/>
       <c r="AY31" s="42"/>
       <c r="AZ31" s="38"/>
       <c r="BA31" s="40"/>
-      <c r="BB31" s="160"/>
-      <c r="BC31" s="160"/>
-      <c r="BD31" s="160"/>
-      <c r="BE31" s="131"/>
-      <c r="BF31" s="81"/>
-      <c r="BG31" s="81"/>
-      <c r="BH31" s="81"/>
-      <c r="BI31" s="81"/>
+      <c r="BB31" s="156"/>
+      <c r="BC31" s="156"/>
+      <c r="BD31" s="156"/>
+      <c r="BE31" s="6"/>
+      <c r="BF31" s="6"/>
+      <c r="BG31" s="6"/>
+      <c r="BH31" s="6"/>
+      <c r="BI31" s="6"/>
       <c r="BJ31" s="39"/>
       <c r="BK31" s="40"/>
       <c r="BL31" s="41"/>
@@ -5321,7 +5301,7 @@
     </row>
     <row r="32" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="194" t="s">
+      <c r="B32" s="186" t="s">
         <v>40</v>
       </c>
       <c r="C32" s="95" t="s">
@@ -5356,7 +5336,7 @@
       <c r="Z32" s="39"/>
       <c r="AA32" s="39"/>
       <c r="AB32" s="40"/>
-      <c r="AC32" s="184"/>
+      <c r="AC32" s="176"/>
       <c r="AD32" s="42"/>
       <c r="AE32" s="38"/>
       <c r="AF32" s="38"/>
@@ -5457,7 +5437,7 @@
       <c r="Z33" s="39"/>
       <c r="AA33" s="39"/>
       <c r="AB33" s="40"/>
-      <c r="AC33" s="184"/>
+      <c r="AC33" s="176"/>
       <c r="AD33" s="42"/>
       <c r="AE33" s="38"/>
       <c r="AF33" s="38"/>
@@ -5522,11 +5502,11 @@
     </row>
     <row r="34" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A34" s="1"/>
-      <c r="B34" s="194" t="s">
+      <c r="B34" s="186" t="s">
         <v>41</v>
       </c>
       <c r="C34" s="95" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D34" s="96">
         <v>45240</v>
@@ -5558,7 +5538,7 @@
       <c r="Z34" s="50"/>
       <c r="AA34" s="50"/>
       <c r="AB34" s="55"/>
-      <c r="AC34" s="190"/>
+      <c r="AC34" s="182"/>
       <c r="AD34" s="57"/>
       <c r="AE34" s="49"/>
       <c r="AF34" s="49"/>
@@ -5587,11 +5567,11 @@
       <c r="BC34" s="50"/>
       <c r="BD34" s="49"/>
       <c r="BE34" s="49"/>
-      <c r="BG34" s="173"/>
-      <c r="BH34" s="172"/>
-      <c r="BI34" s="116"/>
-      <c r="BJ34" s="117"/>
-      <c r="BK34" s="117"/>
+      <c r="BG34" s="165"/>
+      <c r="BH34" s="11"/>
+      <c r="BI34" s="11"/>
+      <c r="BJ34" s="11"/>
+      <c r="BK34" s="11"/>
       <c r="BL34" s="56"/>
       <c r="BM34" s="57"/>
       <c r="BN34" s="49"/>
@@ -5622,7 +5602,7 @@
     </row>
     <row r="35" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="194" t="s">
+      <c r="B35" s="186" t="s">
         <v>42</v>
       </c>
       <c r="C35" s="95" t="s">
@@ -5658,7 +5638,7 @@
       <c r="Z35" s="39"/>
       <c r="AA35" s="39"/>
       <c r="AB35" s="40"/>
-      <c r="AC35" s="184"/>
+      <c r="AC35" s="176"/>
       <c r="AD35" s="42"/>
       <c r="AE35" s="38"/>
       <c r="AF35" s="38"/>
@@ -5688,7 +5668,7 @@
       <c r="BD35" s="38"/>
       <c r="BE35" s="38"/>
       <c r="BF35" s="38"/>
-      <c r="BG35" s="153"/>
+      <c r="BG35" s="149"/>
       <c r="BH35" s="38"/>
       <c r="BI35" s="39"/>
       <c r="BJ35" s="85"/>
@@ -5723,12 +5703,12 @@
     </row>
     <row r="36" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="118" t="s">
+      <c r="B36" s="116" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="119"/>
-      <c r="D36" s="120"/>
-      <c r="E36" s="120"/>
+      <c r="C36" s="117"/>
+      <c r="D36" s="118"/>
+      <c r="E36" s="118"/>
       <c r="F36" s="37"/>
       <c r="G36" s="61"/>
       <c r="H36" s="61"/>
@@ -5749,9 +5729,9 @@
       <c r="W36" s="61"/>
       <c r="X36" s="61"/>
       <c r="Y36" s="61"/>
-      <c r="Z36" s="152"/>
+      <c r="Z36" s="148"/>
       <c r="AA36" s="61"/>
-      <c r="AB36" s="152"/>
+      <c r="AB36" s="148"/>
       <c r="AC36" s="61"/>
       <c r="AD36" s="64"/>
       <c r="AE36" s="61"/>
@@ -5817,16 +5797,16 @@
     </row>
     <row r="37" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A37" s="1"/>
-      <c r="B37" s="195" t="s">
+      <c r="B37" s="187" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="122" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="123">
+      <c r="C37" s="120" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="121">
         <v>45247</v>
       </c>
-      <c r="E37" s="123">
+      <c r="E37" s="121">
         <v>45253</v>
       </c>
       <c r="F37" s="37"/>
@@ -5852,7 +5832,7 @@
       <c r="Z37" s="39"/>
       <c r="AA37" s="39"/>
       <c r="AB37" s="40"/>
-      <c r="AC37" s="184"/>
+      <c r="AC37" s="176"/>
       <c r="AD37" s="42"/>
       <c r="AE37" s="38"/>
       <c r="AF37" s="38"/>
@@ -5890,23 +5870,23 @@
       <c r="BL37" s="41"/>
       <c r="BM37" s="42"/>
       <c r="BN37" s="38"/>
-      <c r="BO37" s="82"/>
-      <c r="BP37" s="82"/>
-      <c r="BQ37" s="82"/>
-      <c r="BR37" s="82"/>
-      <c r="BS37" s="82"/>
-      <c r="BT37" s="107"/>
-      <c r="BU37" s="107"/>
+      <c r="BO37" s="10"/>
+      <c r="BP37" s="10"/>
+      <c r="BQ37" s="10"/>
+      <c r="BR37" s="10"/>
+      <c r="BS37" s="10"/>
+      <c r="BT37" s="10"/>
+      <c r="BU37" s="10"/>
       <c r="BV37" s="38"/>
       <c r="BW37" s="39"/>
       <c r="BX37" s="39"/>
       <c r="BY37" s="79"/>
       <c r="BZ37" s="40"/>
-      <c r="CA37" s="160"/>
-      <c r="CB37" s="160"/>
-      <c r="CC37" s="160"/>
-      <c r="CD37" s="160"/>
-      <c r="CE37" s="160"/>
+      <c r="CA37" s="156"/>
+      <c r="CB37" s="156"/>
+      <c r="CC37" s="156"/>
+      <c r="CD37" s="156"/>
+      <c r="CE37" s="156"/>
       <c r="CG37" s="41"/>
       <c r="CH37" s="105"/>
       <c r="CI37" s="98"/>
@@ -5916,16 +5896,16 @@
     </row>
     <row r="38" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A38" s="1"/>
-      <c r="B38" s="195" t="s">
+      <c r="B38" s="187" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="122" t="s">
+      <c r="C38" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="123">
+      <c r="D38" s="121">
         <v>45247</v>
       </c>
-      <c r="E38" s="123">
+      <c r="E38" s="121">
         <f>D38+2</f>
         <v>45249</v>
       </c>
@@ -5952,7 +5932,7 @@
       <c r="Z38" s="39"/>
       <c r="AA38" s="39"/>
       <c r="AB38" s="40"/>
-      <c r="AC38" s="184"/>
+      <c r="AC38" s="176"/>
       <c r="AD38" s="42"/>
       <c r="AE38" s="38"/>
       <c r="AF38" s="38"/>
@@ -5989,13 +5969,13 @@
       <c r="BK38" s="110"/>
       <c r="BL38" s="111"/>
       <c r="BM38" s="112"/>
-      <c r="BN38" s="177"/>
+      <c r="BN38" s="169"/>
       <c r="BO38" s="103"/>
       <c r="BP38" s="103"/>
       <c r="BQ38" s="103"/>
-      <c r="BR38" s="153"/>
-      <c r="BS38" s="153"/>
-      <c r="BT38" s="153"/>
+      <c r="BR38" s="149"/>
+      <c r="BS38" s="149"/>
+      <c r="BT38" s="149"/>
       <c r="BU38" s="38"/>
       <c r="BV38" s="38"/>
       <c r="BW38" s="39"/>
@@ -6017,16 +5997,16 @@
     </row>
     <row r="39" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A39" s="1"/>
-      <c r="B39" s="121" t="s">
+      <c r="B39" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="122" t="s">
+      <c r="C39" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="123">
+      <c r="D39" s="121">
         <v>45247</v>
       </c>
-      <c r="E39" s="123">
+      <c r="E39" s="121">
         <f t="shared" ref="E39" si="3">D39+3</f>
         <v>45250</v>
       </c>
@@ -6053,7 +6033,7 @@
       <c r="Z39" s="39"/>
       <c r="AA39" s="39"/>
       <c r="AB39" s="40"/>
-      <c r="AC39" s="184"/>
+      <c r="AC39" s="176"/>
       <c r="AD39" s="42"/>
       <c r="AE39" s="38"/>
       <c r="AF39" s="38"/>
@@ -6118,16 +6098,16 @@
     </row>
     <row r="40" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A40" s="1"/>
-      <c r="B40" s="121" t="s">
+      <c r="B40" s="119" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="122" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" s="123">
+      <c r="C40" s="120" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="121">
         <v>45247</v>
       </c>
-      <c r="E40" s="123">
+      <c r="E40" s="121">
         <f>D40+3</f>
         <v>45250</v>
       </c>
@@ -6154,7 +6134,7 @@
       <c r="Z40" s="39"/>
       <c r="AA40" s="39"/>
       <c r="AB40" s="40"/>
-      <c r="AC40" s="184"/>
+      <c r="AC40" s="176"/>
       <c r="AD40" s="42"/>
       <c r="AE40" s="38"/>
       <c r="AF40" s="38"/>
@@ -6192,17 +6172,17 @@
       <c r="BL40" s="41"/>
       <c r="BM40" s="42"/>
       <c r="BN40" s="38"/>
-      <c r="BO40" s="81"/>
-      <c r="BP40" s="81"/>
-      <c r="BQ40" s="81"/>
-      <c r="BR40" s="81"/>
+      <c r="BO40" s="11"/>
+      <c r="BP40" s="11"/>
+      <c r="BQ40" s="11"/>
+      <c r="BR40" s="11"/>
       <c r="BS40" s="79"/>
       <c r="BT40" s="79"/>
       <c r="BU40" s="79"/>
       <c r="BV40" s="40"/>
-      <c r="BW40" s="160"/>
-      <c r="BX40" s="160"/>
-      <c r="BY40" s="160"/>
+      <c r="BW40" s="156"/>
+      <c r="BX40" s="156"/>
+      <c r="BY40" s="156"/>
       <c r="CA40" s="106"/>
       <c r="CB40" s="38"/>
       <c r="CC40" s="38"/>
@@ -6218,16 +6198,16 @@
     </row>
     <row r="41" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A41" s="1"/>
-      <c r="B41" s="195" t="s">
+      <c r="B41" s="187" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="122" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" s="123">
+      <c r="C41" s="120" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" s="121">
         <v>45250</v>
       </c>
-      <c r="E41" s="123">
+      <c r="E41" s="121">
         <f>D41+4</f>
         <v>45254</v>
       </c>
@@ -6254,7 +6234,7 @@
       <c r="Z41" s="39"/>
       <c r="AA41" s="39"/>
       <c r="AB41" s="40"/>
-      <c r="AC41" s="184"/>
+      <c r="AC41" s="176"/>
       <c r="AD41" s="42"/>
       <c r="AE41" s="38"/>
       <c r="AF41" s="38"/>
@@ -6295,11 +6275,11 @@
       <c r="BO41" s="38"/>
       <c r="BP41" s="39"/>
       <c r="BQ41" s="39"/>
-      <c r="BR41" s="81"/>
-      <c r="BS41" s="81"/>
-      <c r="BT41" s="81"/>
-      <c r="BU41" s="133"/>
-      <c r="BV41" s="81"/>
+      <c r="BR41" s="6"/>
+      <c r="BS41" s="6"/>
+      <c r="BT41" s="6"/>
+      <c r="BU41" s="6"/>
+      <c r="BV41" s="6"/>
       <c r="BW41" s="39"/>
       <c r="BX41" s="39"/>
       <c r="BY41" s="79"/>
@@ -6319,16 +6299,16 @@
     </row>
     <row r="42" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A42" s="1"/>
-      <c r="B42" s="195" t="s">
+      <c r="B42" s="187" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="122" t="s">
-        <v>3</v>
-      </c>
-      <c r="D42" s="123">
+      <c r="C42" s="120" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="121">
         <v>45251</v>
       </c>
-      <c r="E42" s="132">
+      <c r="E42" s="129">
         <f>D42+3</f>
         <v>45254</v>
       </c>
@@ -6355,7 +6335,7 @@
       <c r="Z42" s="39"/>
       <c r="AA42" s="39"/>
       <c r="AB42" s="40"/>
-      <c r="AC42" s="184"/>
+      <c r="AC42" s="176"/>
       <c r="AD42" s="42"/>
       <c r="AE42" s="38"/>
       <c r="AF42" s="38"/>
@@ -6392,15 +6372,15 @@
       <c r="BK42" s="40"/>
       <c r="BL42" s="41"/>
       <c r="BM42" s="42"/>
-      <c r="BN42" s="153"/>
-      <c r="BO42" s="153"/>
+      <c r="BN42" s="149"/>
+      <c r="BO42" s="149"/>
       <c r="BP42" s="69"/>
       <c r="BQ42" s="69"/>
-      <c r="BR42" s="130"/>
-      <c r="BS42" s="158"/>
-      <c r="BT42" s="158"/>
-      <c r="BU42" s="158"/>
-      <c r="BV42" s="158"/>
+      <c r="BR42" s="128"/>
+      <c r="BS42" s="154"/>
+      <c r="BT42" s="154"/>
+      <c r="BU42" s="154"/>
+      <c r="BV42" s="154"/>
       <c r="BW42" s="69"/>
       <c r="BX42" s="39"/>
       <c r="BY42" s="79"/>
@@ -6420,16 +6400,16 @@
     </row>
     <row r="43" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A43" s="1"/>
-      <c r="B43" s="195" t="s">
+      <c r="B43" s="187" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="122" t="s">
+      <c r="C43" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="D43" s="123">
+      <c r="D43" s="121">
         <v>45253</v>
       </c>
-      <c r="E43" s="123">
+      <c r="E43" s="121">
         <v>45257</v>
       </c>
       <c r="F43" s="37"/>
@@ -6455,7 +6435,7 @@
       <c r="Z43" s="39"/>
       <c r="AA43" s="39"/>
       <c r="AB43" s="40"/>
-      <c r="AC43" s="184"/>
+      <c r="AC43" s="176"/>
       <c r="AD43" s="42"/>
       <c r="AE43" s="38"/>
       <c r="AF43" s="38"/>
@@ -6492,12 +6472,12 @@
       <c r="BK43" s="40"/>
       <c r="BL43" s="41"/>
       <c r="BM43" s="42"/>
-      <c r="BN43" s="157"/>
-      <c r="BO43" s="157"/>
+      <c r="BN43" s="153"/>
+      <c r="BO43" s="153"/>
       <c r="BP43" s="50"/>
       <c r="BQ43" s="50"/>
       <c r="BR43" s="51"/>
-      <c r="BS43" s="159"/>
+      <c r="BS43" s="155"/>
       <c r="BT43" s="51"/>
       <c r="BU43" s="103"/>
       <c r="BV43" s="103"/>
@@ -6520,16 +6500,16 @@
     </row>
     <row r="44" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A44" s="1"/>
-      <c r="B44" s="195" t="s">
+      <c r="B44" s="187" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="122" t="s">
+      <c r="C44" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="123">
+      <c r="D44" s="121">
         <v>45254</v>
       </c>
-      <c r="E44" s="123">
+      <c r="E44" s="121">
         <v>45257</v>
       </c>
       <c r="F44" s="37"/>
@@ -6555,7 +6535,7 @@
       <c r="Z44" s="39"/>
       <c r="AA44" s="39"/>
       <c r="AB44" s="40"/>
-      <c r="AC44" s="184"/>
+      <c r="AC44" s="176"/>
       <c r="AD44" s="42"/>
       <c r="AE44" s="38"/>
       <c r="AF44" s="38"/>
@@ -6601,9 +6581,9 @@
       <c r="BT44" s="79"/>
       <c r="BU44" s="79"/>
       <c r="BV44" s="82"/>
-      <c r="BW44" s="176"/>
-      <c r="BX44" s="176"/>
-      <c r="BY44" s="176"/>
+      <c r="BW44" s="168"/>
+      <c r="BX44" s="168"/>
+      <c r="BY44" s="168"/>
       <c r="BZ44" s="38"/>
       <c r="CA44" s="38"/>
       <c r="CB44" s="38"/>
@@ -6620,16 +6600,16 @@
     </row>
     <row r="45" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A45" s="1"/>
-      <c r="B45" s="195" t="s">
+      <c r="B45" s="187" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="122" t="s">
+      <c r="C45" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="D45" s="123">
+      <c r="D45" s="121">
         <v>45255</v>
       </c>
-      <c r="E45" s="123">
+      <c r="E45" s="121">
         <f>D45+2</f>
         <v>45257</v>
       </c>
@@ -6656,7 +6636,7 @@
       <c r="Z45" s="39"/>
       <c r="AA45" s="39"/>
       <c r="AB45" s="40"/>
-      <c r="AC45" s="184"/>
+      <c r="AC45" s="176"/>
       <c r="AD45" s="42"/>
       <c r="AE45" s="38"/>
       <c r="AF45" s="38"/>
@@ -6702,9 +6682,9 @@
       <c r="BT45" s="79"/>
       <c r="BU45" s="98"/>
       <c r="BV45" s="38"/>
-      <c r="BW45" s="178"/>
-      <c r="BX45" s="179"/>
-      <c r="BY45" s="180"/>
+      <c r="BW45" s="170"/>
+      <c r="BX45" s="171"/>
+      <c r="BY45" s="172"/>
       <c r="BZ45" s="38"/>
       <c r="CA45" s="38"/>
       <c r="CB45" s="38"/>
@@ -6721,16 +6701,16 @@
     </row>
     <row r="46" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A46" s="1"/>
-      <c r="B46" s="195" t="s">
+      <c r="B46" s="187" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="122" t="s">
+      <c r="C46" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="123">
+      <c r="D46" s="121">
         <v>45259</v>
       </c>
-      <c r="E46" s="123">
+      <c r="E46" s="121">
         <v>45265</v>
       </c>
       <c r="F46" s="37"/>
@@ -6755,8 +6735,8 @@
       <c r="Y46" s="68"/>
       <c r="Z46" s="69"/>
       <c r="AA46" s="69"/>
-      <c r="AB46" s="155"/>
-      <c r="AC46" s="189"/>
+      <c r="AB46" s="151"/>
+      <c r="AC46" s="181"/>
       <c r="AD46" s="74"/>
       <c r="AE46" s="68"/>
       <c r="AF46" s="68"/>
@@ -6790,28 +6770,28 @@
       <c r="BH46" s="68"/>
       <c r="BI46" s="69"/>
       <c r="BJ46" s="69"/>
-      <c r="BK46" s="124"/>
-      <c r="BL46" s="125"/>
-      <c r="BN46" s="160"/>
-      <c r="BO46" s="160"/>
-      <c r="BP46" s="160"/>
-      <c r="BQ46" s="160"/>
-      <c r="BR46" s="160"/>
-      <c r="BS46" s="160"/>
-      <c r="BT46" s="173"/>
-      <c r="BU46" s="156"/>
+      <c r="BK46" s="122"/>
+      <c r="BL46" s="123"/>
+      <c r="BN46" s="156"/>
+      <c r="BO46" s="156"/>
+      <c r="BP46" s="156"/>
+      <c r="BQ46" s="156"/>
+      <c r="BR46" s="156"/>
+      <c r="BS46" s="156"/>
+      <c r="BT46" s="165"/>
+      <c r="BU46" s="152"/>
       <c r="BV46" s="68"/>
       <c r="BW46" s="69"/>
       <c r="BX46" s="69"/>
-      <c r="BY46" s="130"/>
+      <c r="BY46" s="128"/>
       <c r="BZ46" s="68"/>
-      <c r="CA46" s="126"/>
-      <c r="CB46" s="127"/>
-      <c r="CC46" s="127"/>
-      <c r="CD46" s="128"/>
-      <c r="CE46" s="128"/>
-      <c r="CF46" s="129"/>
-      <c r="CG46" s="129"/>
+      <c r="CA46" s="124"/>
+      <c r="CB46" s="125"/>
+      <c r="CC46" s="125"/>
+      <c r="CD46" s="126"/>
+      <c r="CE46" s="126"/>
+      <c r="CF46" s="127"/>
+      <c r="CG46" s="127"/>
       <c r="CH46" s="74"/>
       <c r="CI46" s="68"/>
       <c r="CJ46" s="68"/>
@@ -6820,16 +6800,16 @@
     </row>
     <row r="47" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A47" s="1"/>
-      <c r="B47" s="195" t="s">
+      <c r="B47" s="187" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="122" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" s="123">
+      <c r="C47" s="120" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" s="121">
         <v>45259</v>
       </c>
-      <c r="E47" s="123">
+      <c r="E47" s="121">
         <f>D47+4</f>
         <v>45263</v>
       </c>
@@ -6856,7 +6836,7 @@
       <c r="Z47" s="39"/>
       <c r="AA47" s="39"/>
       <c r="AB47" s="40"/>
-      <c r="AC47" s="184"/>
+      <c r="AC47" s="176"/>
       <c r="AD47" s="42"/>
       <c r="AE47" s="38"/>
       <c r="AF47" s="38"/>
@@ -6892,24 +6872,24 @@
       <c r="BJ47" s="39"/>
       <c r="BK47" s="40"/>
       <c r="BL47" s="41"/>
-      <c r="BN47" s="160"/>
-      <c r="BO47" s="160"/>
-      <c r="BP47" s="160"/>
-      <c r="BQ47" s="160"/>
-      <c r="BR47" s="160"/>
-      <c r="BS47" s="160"/>
-      <c r="BT47" s="160"/>
-      <c r="BU47" s="160"/>
-      <c r="BV47" s="160"/>
-      <c r="BW47" s="160"/>
-      <c r="BX47" s="161"/>
+      <c r="BN47" s="156"/>
+      <c r="BO47" s="156"/>
+      <c r="BP47" s="156"/>
+      <c r="BQ47" s="156"/>
+      <c r="BR47" s="156"/>
+      <c r="BS47" s="156"/>
+      <c r="BT47" s="156"/>
+      <c r="BU47" s="156"/>
+      <c r="BV47" s="156"/>
+      <c r="BW47" s="156"/>
+      <c r="BX47" s="157"/>
       <c r="BY47" s="79"/>
       <c r="BZ47" s="38"/>
-      <c r="CA47" s="172"/>
-      <c r="CB47" s="117"/>
-      <c r="CC47" s="117"/>
-      <c r="CD47" s="117"/>
-      <c r="CE47" s="117"/>
+      <c r="CA47" s="6"/>
+      <c r="CB47" s="6"/>
+      <c r="CC47" s="6"/>
+      <c r="CD47" s="6"/>
+      <c r="CE47" s="6"/>
       <c r="CF47" s="40"/>
       <c r="CG47" s="41"/>
       <c r="CH47" s="42"/>
@@ -6920,16 +6900,16 @@
     </row>
     <row r="48" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A48" s="1"/>
-      <c r="B48" s="195" t="s">
+      <c r="B48" s="187" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="122" t="s">
+      <c r="C48" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="D48" s="123">
+      <c r="D48" s="121">
         <v>45259</v>
       </c>
-      <c r="E48" s="123">
+      <c r="E48" s="121">
         <f>D48+3</f>
         <v>45262</v>
       </c>
@@ -6956,7 +6936,7 @@
       <c r="Z48" s="39"/>
       <c r="AA48" s="39"/>
       <c r="AB48" s="40"/>
-      <c r="AC48" s="184"/>
+      <c r="AC48" s="176"/>
       <c r="AD48" s="42"/>
       <c r="AE48" s="38"/>
       <c r="AF48" s="38"/>
@@ -7006,10 +6986,10 @@
       <c r="BX48" s="39"/>
       <c r="BY48" s="79"/>
       <c r="BZ48" s="38"/>
-      <c r="CA48" s="139"/>
-      <c r="CB48" s="139"/>
-      <c r="CC48" s="139"/>
-      <c r="CD48" s="139"/>
+      <c r="CA48" s="135"/>
+      <c r="CB48" s="135"/>
+      <c r="CC48" s="135"/>
+      <c r="CD48" s="135"/>
       <c r="CE48" s="69"/>
       <c r="CF48" s="83"/>
       <c r="CG48" s="104"/>
@@ -7021,16 +7001,16 @@
     </row>
     <row r="49" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A49" s="1"/>
-      <c r="B49" s="195" t="s">
+      <c r="B49" s="187" t="s">
         <v>52</v>
       </c>
-      <c r="C49" s="122" t="s">
+      <c r="C49" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="D49" s="123">
+      <c r="D49" s="121">
         <v>45260</v>
       </c>
-      <c r="E49" s="123">
+      <c r="E49" s="121">
         <v>45262</v>
       </c>
       <c r="F49" s="37"/>
@@ -7056,7 +7036,7 @@
       <c r="Z49" s="39"/>
       <c r="AA49" s="39"/>
       <c r="AB49" s="40"/>
-      <c r="AC49" s="184"/>
+      <c r="AC49" s="176"/>
       <c r="AD49" s="42"/>
       <c r="AE49" s="38"/>
       <c r="AF49" s="38"/>
@@ -7121,16 +7101,16 @@
     </row>
     <row r="50" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A50" s="1"/>
-      <c r="B50" s="195" t="s">
+      <c r="B50" s="187" t="s">
         <v>53</v>
       </c>
-      <c r="C50" s="122" t="s">
+      <c r="C50" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="D50" s="123">
+      <c r="D50" s="121">
         <v>45262</v>
       </c>
-      <c r="E50" s="123">
+      <c r="E50" s="121">
         <f>D50+3</f>
         <v>45265</v>
       </c>
@@ -7157,7 +7137,7 @@
       <c r="Z50" s="39"/>
       <c r="AA50" s="39"/>
       <c r="AB50" s="40"/>
-      <c r="AC50" s="184"/>
+      <c r="AC50" s="176"/>
       <c r="AD50" s="42"/>
       <c r="AE50" s="38"/>
       <c r="AF50" s="38"/>
@@ -7212,8 +7192,8 @@
       <c r="CC50" s="38"/>
       <c r="CD50" s="75"/>
       <c r="CE50" s="75"/>
-      <c r="CF50" s="134"/>
-      <c r="CG50" s="135"/>
+      <c r="CF50" s="130"/>
+      <c r="CG50" s="131"/>
       <c r="CH50" s="105"/>
       <c r="CI50" s="98"/>
       <c r="CJ50" s="38"/>
@@ -7222,16 +7202,16 @@
     </row>
     <row r="51" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A51" s="1"/>
-      <c r="B51" s="195" t="s">
+      <c r="B51" s="187" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="122" t="s">
+      <c r="C51" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="D51" s="123">
+      <c r="D51" s="121">
         <v>45263</v>
       </c>
-      <c r="E51" s="123">
+      <c r="E51" s="121">
         <f>D51+2</f>
         <v>45265</v>
       </c>
@@ -7258,7 +7238,7 @@
       <c r="Z51" s="39"/>
       <c r="AA51" s="39"/>
       <c r="AB51" s="40"/>
-      <c r="AC51" s="184"/>
+      <c r="AC51" s="176"/>
       <c r="AD51" s="42"/>
       <c r="AE51" s="38"/>
       <c r="AF51" s="38"/>
@@ -7306,15 +7286,15 @@
       <c r="BV51" s="38"/>
       <c r="BW51" s="39"/>
       <c r="BX51" s="39"/>
-      <c r="BY51" s="136"/>
-      <c r="BZ51" s="136"/>
-      <c r="CA51" s="136"/>
+      <c r="BY51" s="132"/>
+      <c r="BZ51" s="132"/>
+      <c r="CA51" s="132"/>
       <c r="CB51" s="106"/>
       <c r="CC51" s="106"/>
       <c r="CD51" s="39"/>
       <c r="CE51" s="85"/>
-      <c r="CF51" s="137"/>
-      <c r="CG51" s="138"/>
+      <c r="CF51" s="133"/>
+      <c r="CG51" s="134"/>
       <c r="CH51" s="105"/>
       <c r="CI51" s="98"/>
       <c r="CJ51" s="38"/>
@@ -7323,97 +7303,97 @@
     </row>
     <row r="52" spans="1:90" ht="15" customHeight="1" thickBot="1">
       <c r="A52" s="1"/>
-      <c r="B52" s="140" t="s">
+      <c r="B52" s="136" t="s">
         <v>27</v>
       </c>
-      <c r="C52" s="141"/>
-      <c r="D52" s="142"/>
-      <c r="E52" s="143"/>
+      <c r="C52" s="137"/>
+      <c r="D52" s="138"/>
+      <c r="E52" s="139"/>
       <c r="F52" s="37"/>
-      <c r="G52" s="144"/>
-      <c r="H52" s="144"/>
-      <c r="I52" s="144"/>
-      <c r="J52" s="144"/>
-      <c r="K52" s="144"/>
-      <c r="L52" s="144"/>
-      <c r="M52" s="144"/>
-      <c r="N52" s="144"/>
-      <c r="O52" s="144"/>
-      <c r="P52" s="144"/>
-      <c r="Q52" s="144"/>
-      <c r="R52" s="144"/>
-      <c r="S52" s="144"/>
-      <c r="T52" s="144"/>
-      <c r="U52" s="144"/>
-      <c r="V52" s="144"/>
-      <c r="W52" s="144"/>
-      <c r="X52" s="144"/>
-      <c r="Y52" s="144"/>
-      <c r="Z52" s="144"/>
-      <c r="AA52" s="144"/>
-      <c r="AB52" s="145"/>
-      <c r="AC52" s="144"/>
-      <c r="AD52" s="147"/>
-      <c r="AE52" s="144"/>
-      <c r="AF52" s="144"/>
-      <c r="AG52" s="144"/>
-      <c r="AH52" s="144"/>
-      <c r="AI52" s="144"/>
-      <c r="AJ52" s="144"/>
-      <c r="AK52" s="144"/>
-      <c r="AL52" s="144"/>
-      <c r="AM52" s="144"/>
-      <c r="AN52" s="144"/>
-      <c r="AO52" s="144"/>
-      <c r="AP52" s="145"/>
-      <c r="AQ52" s="146"/>
-      <c r="AR52" s="147"/>
-      <c r="AS52" s="144"/>
-      <c r="AT52" s="144"/>
-      <c r="AU52" s="144"/>
-      <c r="AV52" s="144"/>
-      <c r="AW52" s="144"/>
-      <c r="AX52" s="144"/>
-      <c r="AY52" s="144"/>
-      <c r="AZ52" s="144"/>
-      <c r="BA52" s="144"/>
-      <c r="BB52" s="144"/>
-      <c r="BC52" s="144"/>
-      <c r="BD52" s="144"/>
-      <c r="BE52" s="144"/>
-      <c r="BF52" s="144"/>
-      <c r="BG52" s="144"/>
-      <c r="BH52" s="144"/>
-      <c r="BI52" s="144"/>
-      <c r="BJ52" s="144"/>
-      <c r="BK52" s="145"/>
-      <c r="BL52" s="146"/>
-      <c r="BM52" s="147"/>
-      <c r="BN52" s="144"/>
-      <c r="BO52" s="144"/>
-      <c r="BP52" s="144"/>
-      <c r="BQ52" s="144"/>
-      <c r="BR52" s="144"/>
-      <c r="BS52" s="144"/>
-      <c r="BT52" s="144"/>
-      <c r="BU52" s="144"/>
-      <c r="BV52" s="144"/>
-      <c r="BW52" s="144"/>
-      <c r="BX52" s="144"/>
-      <c r="BY52" s="144"/>
-      <c r="BZ52" s="144"/>
-      <c r="CA52" s="148"/>
-      <c r="CB52" s="148"/>
-      <c r="CC52" s="148"/>
-      <c r="CD52" s="148"/>
-      <c r="CE52" s="144"/>
-      <c r="CF52" s="145"/>
-      <c r="CG52" s="146"/>
-      <c r="CH52" s="147"/>
-      <c r="CI52" s="144"/>
-      <c r="CJ52" s="144"/>
-      <c r="CK52" s="144"/>
-      <c r="CL52" s="144"/>
+      <c r="G52" s="140"/>
+      <c r="H52" s="140"/>
+      <c r="I52" s="140"/>
+      <c r="J52" s="140"/>
+      <c r="K52" s="140"/>
+      <c r="L52" s="140"/>
+      <c r="M52" s="140"/>
+      <c r="N52" s="140"/>
+      <c r="O52" s="140"/>
+      <c r="P52" s="140"/>
+      <c r="Q52" s="140"/>
+      <c r="R52" s="140"/>
+      <c r="S52" s="140"/>
+      <c r="T52" s="140"/>
+      <c r="U52" s="140"/>
+      <c r="V52" s="140"/>
+      <c r="W52" s="140"/>
+      <c r="X52" s="140"/>
+      <c r="Y52" s="140"/>
+      <c r="Z52" s="140"/>
+      <c r="AA52" s="140"/>
+      <c r="AB52" s="141"/>
+      <c r="AC52" s="140"/>
+      <c r="AD52" s="143"/>
+      <c r="AE52" s="140"/>
+      <c r="AF52" s="140"/>
+      <c r="AG52" s="140"/>
+      <c r="AH52" s="140"/>
+      <c r="AI52" s="140"/>
+      <c r="AJ52" s="140"/>
+      <c r="AK52" s="140"/>
+      <c r="AL52" s="140"/>
+      <c r="AM52" s="140"/>
+      <c r="AN52" s="140"/>
+      <c r="AO52" s="140"/>
+      <c r="AP52" s="141"/>
+      <c r="AQ52" s="142"/>
+      <c r="AR52" s="143"/>
+      <c r="AS52" s="140"/>
+      <c r="AT52" s="140"/>
+      <c r="AU52" s="140"/>
+      <c r="AV52" s="140"/>
+      <c r="AW52" s="140"/>
+      <c r="AX52" s="140"/>
+      <c r="AY52" s="140"/>
+      <c r="AZ52" s="140"/>
+      <c r="BA52" s="140"/>
+      <c r="BB52" s="140"/>
+      <c r="BC52" s="140"/>
+      <c r="BD52" s="140"/>
+      <c r="BE52" s="140"/>
+      <c r="BF52" s="140"/>
+      <c r="BG52" s="140"/>
+      <c r="BH52" s="140"/>
+      <c r="BI52" s="140"/>
+      <c r="BJ52" s="140"/>
+      <c r="BK52" s="141"/>
+      <c r="BL52" s="142"/>
+      <c r="BM52" s="143"/>
+      <c r="BN52" s="140"/>
+      <c r="BO52" s="140"/>
+      <c r="BP52" s="140"/>
+      <c r="BQ52" s="140"/>
+      <c r="BR52" s="140"/>
+      <c r="BS52" s="140"/>
+      <c r="BT52" s="140"/>
+      <c r="BU52" s="140"/>
+      <c r="BV52" s="140"/>
+      <c r="BW52" s="140"/>
+      <c r="BX52" s="140"/>
+      <c r="BY52" s="140"/>
+      <c r="BZ52" s="140"/>
+      <c r="CA52" s="144"/>
+      <c r="CB52" s="144"/>
+      <c r="CC52" s="144"/>
+      <c r="CD52" s="144"/>
+      <c r="CE52" s="140"/>
+      <c r="CF52" s="141"/>
+      <c r="CG52" s="142"/>
+      <c r="CH52" s="143"/>
+      <c r="CI52" s="140"/>
+      <c r="CJ52" s="140"/>
+      <c r="CK52" s="140"/>
+      <c r="CL52" s="140"/>
     </row>
     <row r="53" spans="1:90" ht="30" customHeight="1">
       <c r="A53" s="14"/>
@@ -7421,13 +7401,13 @@
     </row>
     <row r="54" spans="1:90" ht="30" customHeight="1">
       <c r="A54" s="14"/>
-      <c r="C54" s="149"/>
+      <c r="C54" s="145"/>
       <c r="D54" s="7"/>
-      <c r="E54" s="150"/>
+      <c r="E54" s="146"/>
     </row>
     <row r="55" spans="1:90" ht="30" customHeight="1">
       <c r="A55" s="14"/>
-      <c r="C55" s="151"/>
+      <c r="C55" s="147"/>
       <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:90" ht="30" customHeight="1">
@@ -11208,21 +11188,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="I1:P1"/>
-    <mergeCell ref="R1:V1"/>
-    <mergeCell ref="X1:AB1"/>
-    <mergeCell ref="AD1:AK1"/>
-    <mergeCell ref="AM1:AQ1"/>
-    <mergeCell ref="AS1:AV1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="AI4:AO4"/>
-    <mergeCell ref="AP4:AV4"/>
-    <mergeCell ref="AW4:BC4"/>
-    <mergeCell ref="BD4:BJ4"/>
-    <mergeCell ref="BK4:BQ4"/>
-    <mergeCell ref="BR4:BX4"/>
-    <mergeCell ref="BY4:CE4"/>
-    <mergeCell ref="CF4:CL4"/>
     <mergeCell ref="U4:AA4"/>
     <mergeCell ref="AB4:AH4"/>
     <mergeCell ref="D2:E2"/>
@@ -11230,8 +11195,23 @@
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:M4"/>
     <mergeCell ref="N4:T4"/>
+    <mergeCell ref="BD4:BJ4"/>
+    <mergeCell ref="BK4:BQ4"/>
+    <mergeCell ref="BR4:BX4"/>
+    <mergeCell ref="BY4:CE4"/>
+    <mergeCell ref="CF4:CL4"/>
+    <mergeCell ref="AS1:AV1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="AI4:AO4"/>
+    <mergeCell ref="AP4:AV4"/>
+    <mergeCell ref="AW4:BC4"/>
+    <mergeCell ref="I1:P1"/>
+    <mergeCell ref="R1:V1"/>
+    <mergeCell ref="X1:AB1"/>
+    <mergeCell ref="AD1:AK1"/>
+    <mergeCell ref="AM1:AQ1"/>
   </mergeCells>
-  <conditionalFormatting sqref="G5:L9 M5:Y7 Z5:Z6 AD5:AF9 AI5:AM9 AN5:AO6 AP5:AT9 AW5:BA9 BD5:BH9 BK5:BO9 BR5:BV9 CF5:CJ9 BY6:CC9 M9:P9 U9:Z9 AF15:AF16 AI17:AL17 BI5:BJ10 BP5:BQ10 BW5:BW10 CK5:CK10 CD6:CD10 BX7:BX10 CE7:CE10 S9:T10 AP16:AT16 AE14:AF14 AF12:AH13 AC15:AE17 AB13:AE13 U15:Y17 AQ15:AQ16 AR15:AT17 AI11:AT14 G12:Y13 BD12:CL14 AG5:AH13 BD11:CK13 CL7:CL13 BD16:CL16 G11:U13 G16:U16 AB11:AC13 AB16:AK16 Z10:Z13 G14:Z14 Y16:Z16 AG17:AH18 BI15:BJ18 BP15:BQ18 BW15:BX18 CD15:CE18 CK15:CL18 AW32:AW33 G34:K35 N34:R35 BK34:BO35 BR34:BV35 BY34:CC35 CF34:CJ35 BK33:CL33 AB34:AU34 AB33:AV33 AB35:AV35 BB33:BF33 U34:Z35 AB47:BL47 BY47:CE47 CE49:CH49 BW52:BX52 CD52:CE52 AU52:AV52 CK52:CL52 BI52:BJ52 AG52:AH52 AN52:AO52 BP52:BQ52 BK15:BO21 BR15:BV21 BY15:CC21 CF15:CJ21 BG25:CL25 AB26:AV26 BF26:CL26 AW27:AY27 BD27:CL27 G21:Z21 AI18:AT24 AB22:AS24 BB5:BC24 AW11:BA24 AU5:AV24 BD15:BH24 G15:T24 U18:Z24 AB20:AR24 AW28:BA30 AX31:BA31 BJ31:CL31 AY35:BH35 AY34:BE34 BG28:CL30 AW19:CL24 AB24:AV24 AB25:AU25 AB23:CL23 AQ29:AR31 AU32:AV32 AT27:AV30 AX32:CL32 AW29:CL30 AB27:AP32 G23:Z33 BV41:CC44 AB41:BT44 AB40:BQ40 BR38 BP34:BQ36 BS38:BV44 CD48:CG49 AU36:AV36 BB36:BC36 AG36:AH36 AN36:AO36 BI35:BJ36 AB37:BJ40 BW34:BX36 BW37:BY44 BZ37:CC40 CK34:CL36 CD34:CE36 AB37:BZ37 CD37:CL44 CB51:CD51 BV48:CC50 BV51:BX51 CJ48:CL51 CH48:CH51 AB48:BT51 AB45:CL46 G37:K51 N37:R51 U37:Y51 L34:M52 Z37:Z52 S34:T52 AB19:AI24 AB17:AB18 AD18:AF18 AB5:AC7">
+  <conditionalFormatting sqref="G5:L9 M5:Y7 Z5:Z6 AD5:AF9 AI5:AM9 AN5:AO6 AP5:AT9 AW5:BA9 BD5:BH9 BK5:BO9 BR5:BV9 CF5:CJ9 BY6:CC9 M9:P9 U9:Z9 AF15:AF16 AI17:AL17 BI5:BJ10 BP5:BQ10 BW5:BW10 CK5:CK10 CD6:CD10 BX7:BX10 CE7:CE10 S9:T10 AP16:AT16 AE14:AF14 AF12:AH13 AC15:AE17 AB13:AE13 U15:Y17 AQ15:AQ16 AR15:AT17 AI11:AT14 G12:Y13 BD12:CL14 AG5:AH13 BD11:CK13 CL7:CL13 BD16:CL16 G11:U13 G16:U16 AB11:AC13 AB16:AK16 Z10:Z13 G14:Z14 Y16:Z16 AG17:AH18 BI15:BJ18 BP15:BQ18 BW15:BX18 CD15:CE18 CK15:CL18 AW32:AW33 G34:K35 N34:R35 BK35:BO35 BR34:BV35 BY34:CC35 CF34:CJ35 BK33:CL33 AB34:AU34 AB33:AV33 AB35:AV35 BB33:BF33 U34:Z35 AB47:BL47 BY47:BZ47 CE49:CH49 BW52:BX52 CD52:CE52 AU52:AV52 CK52:CL52 BI52:BJ52 AG52:AH52 AN52:AO52 BP52:BQ52 BK15:BO21 BR15:BV21 BY15:CC21 CF15:CJ21 BG25:CL25 AB26:AV26 BF26:CL26 AW27:AY27 BD27:CL27 G21:Z21 AI18:AT24 AB22:AS24 BB5:BC23 AW11:BA23 AU5:AV24 BD15:BH24 G15:T24 U18:Z24 AB20:AR24 AW28:BA30 AX31:BA31 BJ31:CL31 AY35:BH35 AY34:BE34 BG28:CL28 AW19:CL23 AB25:AU25 AB23:CL23 AQ29:AR31 AU32:AV32 AT27:AV30 AX32:CL32 AB27:AP32 G23:Z33 AB40:BN40 BR38 BP34:BQ36 BS38:BV40 CD48:CG49 AU36:AV36 BB36:BC36 AG36:AH36 AN36:AO36 BI35:BJ36 AB37:BJ40 BW34:BX36 BW37:BY44 BZ37:CC40 CK34:CL36 CD34:CE36 AB37:BN37 CD37:CL44 CB51:CD51 BV48:CC50 BV51:BX51 CJ48:CL51 CH48:CH51 AB48:BT51 AB45:CL46 G37:K51 N37:R51 U37:Y51 L34:M52 Z37:Z52 S34:T52 AB19:AI24 AB17:AB18 AD18:AF18 AB5:AC7 AB24:AX24 BD24:CL24 AW30:CL30 AW29:BC29 BK29:CL29 BL34:BO34 BV37:BZ37 BW41:CC41 AB41:BQ41 AB42:CC44">
     <cfRule type="expression" dxfId="21" priority="2">
       <formula>AND(TODAY()&gt;=G$5,TODAY()&lt;H$5)</formula>
     </cfRule>
@@ -11261,12 +11241,12 @@
       <formula>AND(TODAY()&gt;=AN$5,TODAY()&lt;AO$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BD29:BD30 AW30">
+  <conditionalFormatting sqref="BD30 AW30">
     <cfRule type="expression" dxfId="15" priority="10">
       <formula>AND(TODAY()&gt;=AW$5,TODAY()&lt;AX$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BJ29:BK30">
+  <conditionalFormatting sqref="BJ30:BK30 BK29">
     <cfRule type="expression" dxfId="14" priority="11">
       <formula>AND(TODAY()&gt;=BJ$5,TODAY()&lt;BK$5)</formula>
     </cfRule>
@@ -11291,22 +11271,17 @@
       <formula>AND(TODAY()&gt;=CK$5,TODAY()&lt;CL$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CA47:CE47 CD37:CG37 CD46:CG46">
+  <conditionalFormatting sqref="CD37:CG37 CD46:CG46">
     <cfRule type="expression" dxfId="9" priority="17">
-      <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;BN$5)</formula>
+      <formula>AND(TODAY()&gt;=BP$5,TODAY()&lt;BQ$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE31:BI31 AW22:AX24">
+  <conditionalFormatting sqref="AW22:AX24">
     <cfRule type="expression" dxfId="8" priority="21">
       <formula>AND(TODAY()&gt;=AT$5,TODAY()&lt;AU$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AY25:BF25">
-    <cfRule type="expression" dxfId="7" priority="23">
-      <formula>AND(TODAY()&gt;=AV$5,TODAY()&lt;AW$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BF25 AY26:BE26 AY24:BC24">
+  <conditionalFormatting sqref="AY26:BE26">
     <cfRule type="expression" dxfId="6" priority="25">
       <formula>AND(TODAY()&gt;=AW$5,TODAY()&lt;AX$5)</formula>
     </cfRule>
@@ -11316,29 +11291,9 @@
       <formula>AND(TODAY()&gt;=BA$5,TODAY()&lt;BB$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AY24:AZ24">
-    <cfRule type="expression" dxfId="4" priority="36">
-      <formula>AND(TODAY()&gt;=AT$5,TODAY()&lt;AU$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BG34:BK34">
+  <conditionalFormatting sqref="BG34">
     <cfRule type="expression" dxfId="3" priority="38">
       <formula>AND(TODAY()&gt;=BF$5,TODAY()&lt;BG$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BO40:BR40">
-    <cfRule type="expression" dxfId="2" priority="40">
-      <formula>AND(TODAY()&gt;=BW$5,TODAY()&lt;BX$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BO37:BU37">
-    <cfRule type="expression" dxfId="1" priority="42">
-      <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;CB$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BU37">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(TODAY()&gt;=BU$5,TODAY()&lt;BV$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>

</xml_diff>